<commit_message>
add buttons to fullsize card
</commit_message>
<xml_diff>
--- a/cards_info.xlsx
+++ b/cards_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DEV\Unity\Settlers2D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D74E04-38B0-4A82-B2BC-48EEFA66BFF9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C06FB5-89D1-4F84-81B9-BB905D5619EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15675" yWindow="735" windowWidth="24810" windowHeight="13530" xr2:uid="{BA564DFF-F192-4381-993A-0AB2E406A0FA}"/>
+    <workbookView xWindow="21870" yWindow="825" windowWidth="16350" windowHeight="13530" xr2:uid="{BA564DFF-F192-4381-993A-0AB2E406A0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -814,10 +814,10 @@
   <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S10" sqref="S10"/>
+      <selection pane="bottomRight" activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +904,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="str">
-        <f>_xlfn.CONCAT(B$1,B2,C$1,C2,D$1,D2,E$1,E2,F$1,F2,G$1,G2,H$1,H2,I$1,I2,J$1,J2,K$1,K2,L$1)</f>
+        <f t="shared" ref="L2:L33" si="0">_xlfn.CONCAT(B$1,B2,C$1,C2,D$1,D2,E$1,E2,F$1,F2,G$1,G2,H$1,H2,I$1,I2,J$1,J2,K$1,K2,L$1)</f>
         <v>{"cardId":1,"cardName":"STATUA","description":"Cecha: - . Bonus za zbudowanie: 1 #2 za każdą SZARĄ #9 w twoim imperium, maks 6. Dodatkowo dobierz 1 #1.","cardType":8,"fractionType":0,"actionType":2,"contract":0,"cost":[7,8,8],"gain":[2,8],"image":1},</v>
       </c>
     </row>
@@ -943,7 +943,7 @@
         <v>2</v>
       </c>
       <c r="L3" t="str">
-        <f>_xlfn.CONCAT(B$1,B3,C$1,C3,D$1,D3,E$1,E3,F$1,F3,G$1,G3,H$1,H3,I$1,I3,J$1,J3,K$1,K3,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":2,"cardName":"DOSTAWCA","description":"Cecha: Zawsze gdy zbudujesz SZARĄ #9, otrzymujesz 1 #5 i 1 #2.","cardType":8,"fractionType":0,"actionType":2,"contract":0,"cost":[7,8,8],"gain":[5,8],"image":2},</v>
       </c>
     </row>
@@ -982,7 +982,7 @@
         <v>3</v>
       </c>
       <c r="L4" t="str">
-        <f>_xlfn.CONCAT(B$1,B4,C$1,C4,D$1,D4,E$1,E4,F$1,F4,G$1,G4,H$1,H4,I$1,I4,J$1,J4,K$1,K4,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":3,"cardName":"SKŁAD DREWNA","description":"Cecha: - . Bonus za zbudowanie: 1 #2 za każdą BRĄZOWĄ #9 w twoim imperium, maks 6. Dodatkow dobierz 1 #1.","cardType":7,"fractionType":0,"actionType":2,"contract":0,"cost":[7,7,8],"gain":[7,7],"image":3},</v>
       </c>
     </row>
@@ -1021,7 +1021,7 @@
         <v>4</v>
       </c>
       <c r="L5" t="str">
-        <f>_xlfn.CONCAT(B$1,B5,C$1,C5,D$1,D5,E$1,E5,F$1,F5,G$1,G5,H$1,H5,I$1,I5,J$1,J5,K$1,K5,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":4,"cardName":"WARSZTAT STOLARSKI","description":"Cecha: Zawsze gdy zbudujesz BRĄZOWĄ #9, otrzymujesz 1 #5 i 1 #2.","cardType":7,"fractionType":0,"actionType":2,"contract":0,"cost":[7,7,7],"gain":[5,7],"image":4},</v>
       </c>
     </row>
@@ -1060,7 +1060,7 @@
         <v>5</v>
       </c>
       <c r="L6" t="str">
-        <f>_xlfn.CONCAT(B$1,B6,C$1,C6,D$1,D6,E$1,E6,F$1,F6,G$1,G6,H$1,H6,I$1,I6,J$1,J6,K$1,K6,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":5,"cardName":"SZUBIENICA","description":"Cecha: Zawsze gdy plądrujesz, otrzymujesz 1 #2.","cardType":4,"fractionType":0,"actionType":2,"contract":0,"cost":[7,7],"gain":[2,7],"image":5},</v>
       </c>
     </row>
@@ -1099,7 +1099,7 @@
         <v>6</v>
       </c>
       <c r="L7" t="str">
-        <f>_xlfn.CONCAT(B$1,B7,C$1,C7,D$1,D7,E$1,E7,F$1,F7,G$1,G7,H$1,H7,I$1,I7,J$1,J7,K$1,K7,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":6,"cardName":"MŁYN","description":"Cecha: Zawsze gdy zbudujesz CZERWONĄ #9, otrzymujesz 1 #5 i #2.","cardType":6,"fractionType":0,"actionType":2,"contract":0,"cost":[7,7,7],"gain":[3,6],"image":6},</v>
       </c>
     </row>
@@ -1138,7 +1138,7 @@
         <v>7</v>
       </c>
       <c r="L8" t="str">
-        <f>_xlfn.CONCAT(B$1,B8,C$1,C8,D$1,D8,E$1,E8,F$1,F8,G$1,G8,H$1,H8,I$1,I8,J$1,J8,K$1,K8,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":7,"cardName":"STARY LAS","description":"Produkcja: 2 #7.","cardType":7,"fractionType":0,"actionType":1,"contract":0,"cost":[7,7],"gain":[7,7],"image":7},</v>
       </c>
     </row>
@@ -1177,7 +1177,7 @@
         <v>8</v>
       </c>
       <c r="L9" t="str">
-        <f>_xlfn.CONCAT(B$1,B9,C$1,C9,D$1,D9,E$1,E9,F$1,F9,G$1,G9,H$1,H9,I$1,I9,J$1,J9,K$1,K9,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":8,"cardName":"KAMIENIOŁOM","description":"Produkcja: 1 #8. Bonus za zbudowanie: 1 #8","cardType":8,"fractionType":0,"actionType":1,"contract":0,"cost":[7,8],"gain":[8,8],"image":8},</v>
       </c>
     </row>
@@ -1216,7 +1216,7 @@
         <v>8</v>
       </c>
       <c r="L10" t="str">
-        <f>_xlfn.CONCAT(B$1,B10,C$1,C10,D$1,D10,E$1,E10,F$1,F10,G$1,G10,H$1,H10,I$1,I10,J$1,J10,K$1,K10,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":9,"cardName":"KAMIENIOŁOM","description":"Produkcja: 1 #8. Bonus za zbudowanie: 1 #8","cardType":8,"fractionType":0,"actionType":1,"contract":0,"cost":[7,8],"gain":[8,8],"image":8},</v>
       </c>
     </row>
@@ -1255,7 +1255,7 @@
         <v>8</v>
       </c>
       <c r="L11" t="str">
-        <f>_xlfn.CONCAT(B$1,B11,C$1,C11,D$1,D11,E$1,E11,F$1,F11,G$1,G11,H$1,H11,I$1,I11,J$1,J11,K$1,K11,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":10,"cardName":"KAMIENIOŁOM","description":"Produkcja: 1 #8. Bonus za zbudowanie: 1 #8","cardType":8,"fractionType":0,"actionType":1,"contract":0,"cost":[7,8],"gain":[8,8],"image":8},</v>
       </c>
     </row>
@@ -1294,7 +1294,7 @@
         <v>11</v>
       </c>
       <c r="L12" t="str">
-        <f>_xlfn.CONCAT(B$1,B12,C$1,C12,D$1,D12,E$1,E12,F$1,F12,G$1,G12,H$1,H12,I$1,I12,J$1,J12,K$1,K12,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":11,"cardName":"GRUZOWISKO","description":"Produkcja: 1 #8 za każdą Szarą #9 w twoim imperium, maks. 3.","cardType":8,"fractionType":0,"actionType":1,"contract":0,"cost":[7,7,8],"gain":[8,8],"image":11},</v>
       </c>
     </row>
@@ -1333,7 +1333,7 @@
         <v>12</v>
       </c>
       <c r="L13" t="str">
-        <f>_xlfn.CONCAT(B$1,B13,C$1,C13,D$1,D13,E$1,E13,F$1,F13,G$1,G13,H$1,H13,I$1,I13,J$1,J13,K$1,K13,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":12,"cardName":"WIOSKA","description":"Produkcja: 1 #3. Bonus za zbudowanie: 1 #3","cardType":3,"fractionType":0,"actionType":1,"contract":0,"cost":[7],"gain":[3,3],"image":12},</v>
       </c>
     </row>
@@ -1372,7 +1372,7 @@
         <v>12</v>
       </c>
       <c r="L14" t="str">
-        <f>_xlfn.CONCAT(B$1,B14,C$1,C14,D$1,D14,E$1,E14,F$1,F14,G$1,G14,H$1,H14,I$1,I14,J$1,J14,K$1,K14,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":13,"cardName":"WIOSKA","description":"Produkcja: 1 #3. Bonus za zbudowanie: 1 #3","cardType":3,"fractionType":0,"actionType":1,"contract":0,"cost":[7],"gain":[3,3],"image":12},</v>
       </c>
     </row>
@@ -1411,7 +1411,7 @@
         <v>12</v>
       </c>
       <c r="L15" t="str">
-        <f>_xlfn.CONCAT(B$1,B15,C$1,C15,D$1,D15,E$1,E15,F$1,F15,G$1,G15,H$1,H15,I$1,I15,J$1,J15,K$1,K15,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":14,"cardName":"WIOSKA","description":"Produkcja: 1 #3. Bonus za zbudowanie: 1 #3","cardType":3,"fractionType":0,"actionType":1,"contract":0,"cost":[7],"gain":[3,3],"image":12},</v>
       </c>
     </row>
@@ -1450,7 +1450,7 @@
         <v>15</v>
       </c>
       <c r="L16" t="str">
-        <f>_xlfn.CONCAT(B$1,B16,C$1,C16,D$1,D16,E$1,E16,F$1,F16,G$1,G16,H$1,H16,I$1,I16,J$1,J16,K$1,K16,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":15,"cardName":"MIASTECZKO","description":"Produkcja: 2 #3.","cardType":3,"fractionType":0,"actionType":1,"contract":0,"cost":[7,8],"gain":[3,3],"image":15},</v>
       </c>
     </row>
@@ -1489,7 +1489,7 @@
         <v>16</v>
       </c>
       <c r="L17" t="str">
-        <f>_xlfn.CONCAT(B$1,B17,C$1,C17,D$1,D17,E$1,E17,F$1,F17,G$1,G17,H$1,H17,I$1,I17,J$1,J17,K$1,K17,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":16,"cardName":"ROLNICY PRZY PRACY","description":"Produkcja: Wybierz inną ze swoich #9 PRODUKCYJNYCH i orzymaj Dobra, których ona dostarcza. Bonus za zbudowanie: 1 #1.","cardType":3,"fractionType":0,"actionType":1,"contract":0,"cost":[7,7,7],"gain":[3,5],"image":16},</v>
       </c>
     </row>
@@ -1528,7 +1528,7 @@
         <v>17</v>
       </c>
       <c r="L18" t="str">
-        <f>_xlfn.CONCAT(B$1,B18,C$1,C18,D$1,D18,E$1,E18,F$1,F18,G$1,G18,H$1,H18,I$1,I18,J$1,J18,K$1,K18,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":17,"cardName":"ŁAŹNIA U MAMUŚKI","description":"Produkcja: 1 #3 za każdą RÓŻOWĄ #9 w twoim imperium, maks 3.","cardType":3,"fractionType":0,"actionType":1,"contract":0,"cost":[7,7,8],"gain":[3,6],"image":17},</v>
       </c>
     </row>
@@ -1567,7 +1567,7 @@
         <v>18</v>
       </c>
       <c r="L19" t="str">
-        <f>_xlfn.CONCAT(B$1,B19,C$1,C19,D$1,D19,E$1,E19,F$1,F19,G$1,G19,H$1,H19,I$1,I19,J$1,J19,K$1,K19,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":18,"cardName":"PŁATNERZ","description":"Produkcja: 1 #4.","cardType":4,"fractionType":0,"actionType":1,"contract":0,"cost":[7,8],"gain":[2,8],"image":18},</v>
       </c>
     </row>
@@ -1606,7 +1606,7 @@
         <v>18</v>
       </c>
       <c r="L20" t="str">
-        <f>_xlfn.CONCAT(B$1,B20,C$1,C20,D$1,D20,E$1,E20,F$1,F20,G$1,G20,H$1,H20,I$1,I20,J$1,J20,K$1,K20,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":19,"cardName":"PŁATNERZ","description":"Produkcja: 1 #4.","cardType":4,"fractionType":0,"actionType":1,"contract":0,"cost":[7,8],"gain":[2,8],"image":18},</v>
       </c>
     </row>
@@ -1645,7 +1645,7 @@
         <v>18</v>
       </c>
       <c r="L21" t="str">
-        <f>_xlfn.CONCAT(B$1,B21,C$1,C21,D$1,D21,E$1,E21,F$1,F21,G$1,G21,H$1,H21,I$1,I21,J$1,J21,K$1,K21,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":20,"cardName":"PŁATNERZ","description":"Produkcja: 1 #4.","cardType":4,"fractionType":0,"actionType":1,"contract":0,"cost":[7,8],"gain":[2,8],"image":18},</v>
       </c>
     </row>
@@ -1684,7 +1684,7 @@
         <v>21</v>
       </c>
       <c r="L22" t="str">
-        <f>_xlfn.CONCAT(B$1,B22,C$1,C22,D$1,D22,E$1,E22,F$1,F22,G$1,G22,H$1,H22,I$1,I22,J$1,J22,K$1,K22,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":21,"cardName":"KOPALNIA ZŁOTA","description":"Akcja: Wydaj 1 #3, aby dobrać 1 #5. Możesz aktywować jż dwa razy.","cardType":5,"fractionType":0,"actionType":3,"contract":0,"cost":[7,8],"gain":[2,5],"image":21},</v>
       </c>
     </row>
@@ -1723,7 +1723,7 @@
         <v>21</v>
       </c>
       <c r="L23" t="str">
-        <f>_xlfn.CONCAT(B$1,B23,C$1,C23,D$1,D23,E$1,E23,F$1,F23,G$1,G23,H$1,H23,I$1,I23,J$1,J23,K$1,K23,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":22,"cardName":"KOPALNIA ZŁOTA","description":"Akcja: Wydaj 1 #3, aby dobrać 1 #5. Możesz aktywować jż dwa razy.","cardType":5,"fractionType":0,"actionType":3,"contract":0,"cost":[7,8],"gain":[2,5],"image":21},</v>
       </c>
     </row>
@@ -1762,7 +1762,7 @@
         <v>23</v>
       </c>
       <c r="L24" t="str">
-        <f>_xlfn.CONCAT(B$1,B24,C$1,C24,D$1,D24,E$1,E24,F$1,F24,G$1,G24,H$1,H24,I$1,I24,J$1,J24,K$1,K24,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":23,"cardName":"POLE PRZENICY","description":"Produkcja: 1 #6. Bonus za zbudowanie: 1 #6.","cardType":6,"fractionType":0,"actionType":1,"contract":0,"cost":[7,6],"gain":[6,6],"image":23},</v>
       </c>
     </row>
@@ -1801,7 +1801,7 @@
         <v>23</v>
       </c>
       <c r="L25" t="str">
-        <f>_xlfn.CONCAT(B$1,B25,C$1,C25,D$1,D25,E$1,E25,F$1,F25,G$1,G25,H$1,H25,I$1,I25,J$1,J25,K$1,K25,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":24,"cardName":"POLE PRZENICY","description":"Produkcja: 1 #6. Bonus za zbudowanie: 1 #6.","cardType":6,"fractionType":0,"actionType":1,"contract":0,"cost":[7,6],"gain":[6,6],"image":23},</v>
       </c>
     </row>
@@ -1840,7 +1840,7 @@
         <v>25</v>
       </c>
       <c r="L26" t="str">
-        <f>_xlfn.CONCAT(B$1,B26,C$1,C26,D$1,D26,E$1,E26,F$1,F26,G$1,G26,H$1,H26,I$1,I26,J$1,J26,K$1,K26,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":25,"cardName":"SZLACHECKIE POLE","description":"Produkcja: 1 #6 za każdą CZERWONĄ #9 w twoim imperium, maks. 3.","cardType":6,"fractionType":0,"actionType":1,"contract":0,"cost":[7,7,8],"gain":[6,6],"image":25},</v>
       </c>
     </row>
@@ -1879,7 +1879,7 @@
         <v>26</v>
       </c>
       <c r="L27" t="str">
-        <f>_xlfn.CONCAT(B$1,B27,C$1,C27,D$1,D27,E$1,E27,F$1,F27,G$1,G27,H$1,H27,I$1,I27,J$1,J27,K$1,K27,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":26,"cardName":"POMNIK","description":"Produkcja: 1 #2.","cardType":2,"fractionType":0,"actionType":1,"contract":0,"cost":[8],"gain":[2,8],"image":26},</v>
       </c>
     </row>
@@ -1918,7 +1918,7 @@
         <v>27</v>
       </c>
       <c r="L28" t="str">
-        <f>_xlfn.CONCAT(B$1,B28,C$1,C28,D$1,D28,E$1,E28,F$1,F28,G$1,G28,H$1,H28,I$1,I28,J$1,J28,K$1,K28,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":27,"cardName":"GILDIA KUPCÓW","description":"Produkcja: 1 #5 za każdą ZŁOTĄ #9 w twoim imperium, maks 3.","cardType":5,"fractionType":0,"actionType":1,"contract":0,"cost":[7,7,8],"gain":[5,8],"image":27},</v>
       </c>
     </row>
@@ -1957,7 +1957,7 @@
         <v>28</v>
       </c>
       <c r="L29" t="str">
-        <f>_xlfn.CONCAT(B$1,B29,C$1,C29,D$1,D29,E$1,E29,F$1,F29,G$1,G29,H$1,H29,I$1,I29,J$1,J29,K$1,K29,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":28,"cardName":"ZŁOTY POTOK","description":"Produkcja: 1 #5.","cardType":5,"fractionType":0,"actionType":1,"contract":0,"cost":[7,8],"gain":[5,3],"image":28},</v>
       </c>
     </row>
@@ -1996,7 +1996,7 @@
         <v>29</v>
       </c>
       <c r="L30" t="str">
-        <f>_xlfn.CONCAT(B$1,B30,C$1,C30,D$1,D30,E$1,E30,F$1,F30,G$1,G30,H$1,H30,I$1,I30,J$1,J30,K$1,K30,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":29,"cardName":"DOSTAWCA DREWNA","description":"Produkcja: 1 #7 za każdą BRĄZOWĄ #9 w towim imperium, maks 3.","cardType":7,"fractionType":0,"actionType":1,"contract":0,"cost":[7,7,7],"gain":[7,7],"image":29},</v>
       </c>
     </row>
@@ -2035,7 +2035,7 @@
         <v>30</v>
       </c>
       <c r="L31" t="str">
-        <f>_xlfn.CONCAT(B$1,B31,C$1,C31,D$1,D31,E$1,E31,F$1,F31,G$1,G31,H$1,H31,I$1,I31,J$1,J31,K$1,K31,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":30,"cardName":"ZAKŁAD ZŁOTNICZY","description":"Akcja: Wydaj 1 #3 i 1 #5, aby otrzymać 2 #2.","cardType":5,"fractionType":0,"actionType":3,"contract":0,"cost":[7,8],"gain":[2,5],"image":30},</v>
       </c>
     </row>
@@ -2074,7 +2074,7 @@
         <v>30</v>
       </c>
       <c r="L32" t="str">
-        <f>_xlfn.CONCAT(B$1,B32,C$1,C32,D$1,D32,E$1,E32,F$1,F32,G$1,G32,H$1,H32,I$1,I32,J$1,J32,K$1,K32,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":31,"cardName":"ZAKŁAD ZŁOTNICZY","description":"Akcja: Wydaj 1 #3 i 1 #5, aby otrzymać 2 #2.","cardType":5,"fractionType":0,"actionType":3,"contract":0,"cost":[7,8],"gain":[2,5],"image":30},</v>
       </c>
     </row>
@@ -2113,7 +2113,7 @@
         <v>32</v>
       </c>
       <c r="L33" t="str">
-        <f>_xlfn.CONCAT(B$1,B33,C$1,C33,D$1,D33,E$1,E33,F$1,F33,G$1,G33,H$1,H33,I$1,I33,J$1,J33,K$1,K33,L$1)</f>
+        <f t="shared" si="0"/>
         <v>{"cardId":32,"cardName":"JARMARK","description":"Akcja: Wydaj 1 #7, 1 #8 i 1 #6, aby otrzymać 3 #2.","cardType":5,"fractionType":0,"actionType":3,"contract":0,"cost":[7,7],"gain":[5,7],"image":32},</v>
       </c>
     </row>
@@ -2152,7 +2152,7 @@
         <v>33</v>
       </c>
       <c r="L34" t="str">
-        <f>_xlfn.CONCAT(B$1,B34,C$1,C34,D$1,D34,E$1,E34,F$1,F34,G$1,G34,H$1,H34,I$1,I34,J$1,J34,K$1,K34,L$1)</f>
+        <f t="shared" ref="L34:L65" si="1">_xlfn.CONCAT(B$1,B34,C$1,C34,D$1,D34,E$1,E34,F$1,F34,G$1,G34,H$1,H34,I$1,I34,J$1,J34,K$1,K34,L$1)</f>
         <v>{"cardId":33,"cardName":"KOPALNIA WĘGLA","description":"Akcja: Wydaj 1 #3, aby otrzymać 2 #8.","cardType":8,"fractionType":0,"actionType":3,"contract":0,"cost":[7,8],"gain":[3,8],"image":33},</v>
       </c>
     </row>
@@ -2191,7 +2191,7 @@
         <v>34</v>
       </c>
       <c r="L35" t="str">
-        <f>_xlfn.CONCAT(B$1,B35,C$1,C35,D$1,D35,E$1,E35,F$1,F35,G$1,G35,H$1,H35,I$1,I35,J$1,J35,K$1,K35,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":34,"cardName":"MURARZ","description":"Akcja: Wydaj 1 #3 i 1 #8, aby otrzymać 2 #2.","cardType":8,"fractionType":0,"actionType":3,"contract":0,"cost":[7,8],"gain":[7,8],"image":34},</v>
       </c>
     </row>
@@ -2230,7 +2230,7 @@
         <v>34</v>
       </c>
       <c r="L36" t="str">
-        <f>_xlfn.CONCAT(B$1,B36,C$1,C36,D$1,D36,E$1,E36,F$1,F36,G$1,G36,H$1,H36,I$1,I36,J$1,J36,K$1,K36,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":35,"cardName":"MURARZ","description":"Akcja: Wydaj 1 #3 i 1 #8, aby otrzymać 2 #2.","cardType":8,"fractionType":0,"actionType":3,"contract":0,"cost":[8,8],"gain":[2,8],"image":34},</v>
       </c>
     </row>
@@ -2269,7 +2269,7 @@
         <v>36</v>
       </c>
       <c r="L37" t="str">
-        <f>_xlfn.CONCAT(B$1,B37,C$1,C37,D$1,D37,E$1,E37,F$1,F37,G$1,G37,H$1,H37,I$1,I37,J$1,J37,K$1,K37,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":36,"cardName":"NADWORNY RZEŹBIARZ","description":"Akcja: Wydaj 1 #8, aby otrzymać 1 #2. Możesz aktywować ją dwa razy.","cardType":8,"fractionType":0,"actionType":3,"contract":0,"cost":[8],"gain":[3,8],"image":36},</v>
       </c>
     </row>
@@ -2308,7 +2308,7 @@
         <v>37</v>
       </c>
       <c r="L38" t="str">
-        <f>_xlfn.CONCAT(B$1,B38,C$1,C38,D$1,D38,E$1,E38,F$1,F38,G$1,G38,H$1,H38,I$1,I38,J$1,J38,K$1,K38,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":37,"cardName":"CECH MURARZY","description":"Akcja: Wydaj 1 #3 i 2 #8, aby otrzymać 3 #2.","cardType":8,"fractionType":0,"actionType":3,"contract":0,"cost":[7,7,8],"gain":[5,8],"image":37},</v>
       </c>
     </row>
@@ -2347,7 +2347,7 @@
         <v>37</v>
       </c>
       <c r="L39" t="str">
-        <f>_xlfn.CONCAT(B$1,B39,C$1,C39,D$1,D39,E$1,E39,F$1,F39,G$1,G39,H$1,H39,I$1,I39,J$1,J39,K$1,K39,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":38,"cardName":"CECH MURARZY","description":"Akcja: Wydaj 1 #3 i 2 #8, aby otrzymać 3 #2.","cardType":8,"fractionType":0,"actionType":3,"contract":0,"cost":[7,7,8],"gain":[5,8],"image":37},</v>
       </c>
     </row>
@@ -2386,7 +2386,7 @@
         <v>39</v>
       </c>
       <c r="L40" t="str">
-        <f>_xlfn.CONCAT(B$1,B40,C$1,C40,D$1,D40,E$1,E40,F$1,F40,G$1,G40,H$1,H40,I$1,I40,J$1,J40,K$1,K40,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":39,"cardName":"MISJONARZE","description":"Akcja: Wydaj 1 #3 i 1 #4, aby otrzymać 3 #2.","cardType":3,"fractionType":0,"actionType":3,"contract":0,"cost":[6,6],"gain":[2,3],"image":39},</v>
       </c>
     </row>
@@ -2425,7 +2425,7 @@
         <v>40</v>
       </c>
       <c r="L41" t="str">
-        <f>_xlfn.CONCAT(B$1,B41,C$1,C41,D$1,D41,E$1,E41,F$1,F41,G$1,G41,H$1,H41,I$1,I41,J$1,J41,K$1,K41,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":40,"cardName":"OSADNICY","description":"Akcja: Wydaj 1 #7, aby natychmiast zbudować #9 FRAKCYJNĄ, ignorując #9 w kosztach budowy.","cardType":3,"fractionType":0,"actionType":3,"contract":0,"cost":[7],"gain":[3,7],"image":40},</v>
       </c>
     </row>
@@ -2464,7 +2464,7 @@
         <v>41</v>
       </c>
       <c r="L42" t="str">
-        <f>_xlfn.CONCAT(B$1,B42,C$1,C42,D$1,D42,E$1,E42,F$1,F42,G$1,G42,H$1,H42,I$1,I42,J$1,J42,K$1,K42,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":41,"cardName":"TRUPA","description":"Akcja: Wydaj 1 #3, aby wybrać inną ze swoich #9 z AKCJĄ. Usuń z niej dobra wydane na jej aktywację. Możesz ponownie aktywować tamtą #9.","cardType":3,"fractionType":0,"actionType":3,"contract":0,"cost":[7,7],"gain":[3,7],"image":41},</v>
       </c>
     </row>
@@ -2503,7 +2503,7 @@
         <v>42</v>
       </c>
       <c r="L43" t="str">
-        <f>_xlfn.CONCAT(B$1,B43,C$1,C43,D$1,D43,E$1,E43,F$1,F43,G$1,G43,H$1,H43,I$1,I43,J$1,J43,K$1,K43,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":42,"cardName":"DRWALE","description":"Akcja: Wydaj 1 #3, aby otrzymać 2 #7.","cardType":7,"fractionType":0,"actionType":3,"contract":0,"cost":[7,7],"gain":[7,7],"image":42},</v>
       </c>
     </row>
@@ -2542,7 +2542,7 @@
         <v>43</v>
       </c>
       <c r="L44" t="str">
-        <f>_xlfn.CONCAT(B$1,B44,C$1,C44,D$1,D44,E$1,E44,F$1,F44,G$1,G44,H$1,H44,I$1,I44,J$1,J44,K$1,K44,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":43,"cardName":"STOLARZ","description":"Akcja: Wydaj 1 #3 i 2 #7, aby otrzymać 3 #2.","cardType":7,"fractionType":0,"actionType":3,"contract":0,"cost":[7,7,8],"gain":[2,7],"image":43},</v>
       </c>
     </row>
@@ -2581,7 +2581,7 @@
         <v>44</v>
       </c>
       <c r="L45" t="str">
-        <f>_xlfn.CONCAT(B$1,B45,C$1,C45,D$1,D45,E$1,E45,F$1,F45,G$1,G45,H$1,H45,I$1,I45,J$1,J45,K$1,K45,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":44,"cardName":"CIEŚLA","description":"Akcja: Wydaj 1 #3 i 1 #7, aby otrzymać 2 #2.","cardType":7,"fractionType":0,"actionType":3,"contract":0,"cost":[7,7],"gain":[2,7],"image":44},</v>
       </c>
     </row>
@@ -2620,7 +2620,7 @@
         <v>44</v>
       </c>
       <c r="L46" t="str">
-        <f>_xlfn.CONCAT(B$1,B46,C$1,C46,D$1,D46,E$1,E46,F$1,F46,G$1,G46,H$1,H46,I$1,I46,J$1,J46,K$1,K46,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":45,"cardName":"CIEŚLA","description":"Akcja: Wydaj 1 #3 i 1 #7, aby otrzymać 2 #2.","cardType":7,"fractionType":0,"actionType":3,"contract":0,"cost":[7,7],"gain":[2,7],"image":44},</v>
       </c>
     </row>
@@ -2659,7 +2659,7 @@
         <v>46</v>
       </c>
       <c r="L47" t="str">
-        <f>_xlfn.CONCAT(B$1,B47,C$1,C47,D$1,D47,E$1,E47,F$1,F47,G$1,G47,H$1,H47,I$1,I47,J$1,J47,K$1,K47,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":46,"cardName":"ZAMEK","description":"Akcja: Wydaj 1 #3, aby dobrać 1 #1. Możesz aktywować jż dwa razy.","cardType":1,"fractionType":0,"actionType":3,"contract":0,"cost":[7,8],"gain":[1,1],"image":46},</v>
       </c>
     </row>
@@ -2698,7 +2698,7 @@
         <v>46</v>
       </c>
       <c r="L48" t="str">
-        <f>_xlfn.CONCAT(B$1,B48,C$1,C48,D$1,D48,E$1,E48,F$1,F48,G$1,G48,H$1,H48,I$1,I48,J$1,J48,K$1,K48,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":47,"cardName":"ZAMEK","description":"Akcja: Wydaj 1 #3, aby dobrać 1 #1. Możesz aktywować jż dwa razy.","cardType":1,"fractionType":0,"actionType":3,"contract":0,"cost":[7,8],"gain":[1,1],"image":46},</v>
       </c>
     </row>
@@ -2737,7 +2737,7 @@
         <v>46</v>
       </c>
       <c r="L49" t="str">
-        <f>_xlfn.CONCAT(B$1,B49,C$1,C49,D$1,D49,E$1,E49,F$1,F49,G$1,G49,H$1,H49,I$1,I49,J$1,J49,K$1,K49,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":48,"cardName":"ZAMEK","description":"Akcja: Wydaj 1 #3, aby dobrać 1 #1. Możesz aktywować jż dwa razy.","cardType":1,"fractionType":0,"actionType":3,"contract":0,"cost":[8,8],"gain":[1,1],"image":46},</v>
       </c>
     </row>
@@ -2776,7 +2776,7 @@
         <v>49</v>
       </c>
       <c r="L50" t="str">
-        <f>_xlfn.CONCAT(B$1,B50,C$1,C50,D$1,D50,E$1,E50,F$1,F50,G$1,G50,H$1,H50,I$1,I50,J$1,J50,K$1,K50,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":49,"cardName":"TAWERNA","description":"Akcja: Odrzuć 1 #1 z ręki, aby otrzymać 2 #2. Bonus za zbudowanie: 1 #1.","cardType":1,"fractionType":0,"actionType":3,"contract":0,"cost":[7,8],"gain":[1,1],"image":49},</v>
       </c>
     </row>
@@ -2815,7 +2815,7 @@
         <v>50</v>
       </c>
       <c r="L51" t="str">
-        <f>_xlfn.CONCAT(B$1,B51,C$1,C51,D$1,D51,E$1,E51,F$1,F51,G$1,G51,H$1,H51,I$1,I51,J$1,J51,K$1,K51,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":50,"cardName":"KOSZARY","description":"Akcja: Wydaj 1 #3, aby otzrymać 1 #4. Możesz aktywować ją dwa razy.","cardType":4,"fractionType":0,"actionType":3,"contract":0,"cost":[7,8,8],"gain":[2,3],"image":50},</v>
       </c>
     </row>
@@ -2854,7 +2854,7 @@
         <v>50</v>
       </c>
       <c r="L52" t="str">
-        <f>_xlfn.CONCAT(B$1,B52,C$1,C52,D$1,D52,E$1,E52,F$1,F52,G$1,G52,H$1,H52,I$1,I52,J$1,J52,K$1,K52,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":51,"cardName":"KOSZARY","description":"Akcja: Wydaj 1 #3, aby otzrymać 1 #4. Możesz aktywować ją dwa razy.","cardType":4,"fractionType":0,"actionType":3,"contract":0,"cost":[7,8,8],"gain":[2,3],"image":50},</v>
       </c>
     </row>
@@ -2893,7 +2893,7 @@
         <v>52</v>
       </c>
       <c r="L53" t="str">
-        <f>_xlfn.CONCAT(B$1,B53,C$1,C53,D$1,D53,E$1,E53,F$1,F53,G$1,G53,H$1,H53,I$1,I53,J$1,J53,K$1,K53,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":52,"cardName":"CUKIERNIK","description":"Akcja: Wydaj 1 #3 i 2 #6, aby otrzymać 3 #2.","cardType":6,"fractionType":0,"actionType":3,"contract":0,"cost":[7,7,8],"gain":[5,6],"image":52},</v>
       </c>
     </row>
@@ -2932,7 +2932,7 @@
         <v>53</v>
       </c>
       <c r="L54" t="str">
-        <f>_xlfn.CONCAT(B$1,B54,C$1,C54,D$1,D54,E$1,E54,F$1,F54,G$1,G54,H$1,H54,I$1,I54,J$1,J54,K$1,K54,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":53,"cardName":"HODOWCA ŚWIŃ","description":"Akcja: Wydaj 1 #3 i 1 #6, aby otrzymać 2 #2.","cardType":6,"fractionType":0,"actionType":3,"contract":0,"cost":[7,8],"gain":[3,6],"image":53},</v>
       </c>
     </row>
@@ -2971,7 +2971,7 @@
         <v>53</v>
       </c>
       <c r="L55" t="str">
-        <f>_xlfn.CONCAT(B$1,B55,C$1,C55,D$1,D55,E$1,E55,F$1,F55,G$1,G55,H$1,H55,I$1,I55,J$1,J55,K$1,K55,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":54,"cardName":"HODOWCA ŚWIŃ","description":"Akcja: Wydaj 1 #3 i 1 #6, aby otrzymać 2 #2.","cardType":6,"fractionType":0,"actionType":3,"contract":0,"cost":[7,8],"gain":[3,6],"image":53},</v>
       </c>
     </row>
@@ -3010,7 +3010,7 @@
         <v>53</v>
       </c>
       <c r="L56" t="str">
-        <f>_xlfn.CONCAT(B$1,B56,C$1,C56,D$1,D56,E$1,E56,F$1,F56,G$1,G56,H$1,H56,I$1,I56,J$1,J56,K$1,K56,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":55,"cardName":"HODOWCA ŚWIŃ","description":"Akcja: Wydaj 1 #3 i 1 #6, aby otrzymać 2 #2.","cardType":6,"fractionType":0,"actionType":3,"contract":0,"cost":[7,8],"gain":[3,6],"image":53},</v>
       </c>
     </row>
@@ -3049,7 +3049,7 @@
         <v>56</v>
       </c>
       <c r="L57" t="str">
-        <f>_xlfn.CONCAT(B$1,B57,C$1,C57,D$1,D57,E$1,E57,F$1,F57,G$1,G57,H$1,H57,I$1,I57,J$1,J57,K$1,K57,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":56,"cardName":"PIWOWAR","description":"Akcja: Wydaj 1 #6, aby otrzymać 1 #2. Możesz aktywować ją dwa razy.","cardType":6,"fractionType":0,"actionType":3,"contract":0,"cost":[7],"gain":[7,6],"image":56},</v>
       </c>
     </row>
@@ -3088,7 +3088,7 @@
         <v>57</v>
       </c>
       <c r="L58" t="str">
-        <f>_xlfn.CONCAT(B$1,B58,C$1,C58,D$1,D58,E$1,E58,F$1,F58,G$1,G58,H$1,H58,I$1,I58,J$1,J58,K$1,K58,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":57,"cardName":"CESARSKI POSŁANIEC","description":"Akcja: Wydaj 1 #3, aby wybrać jedną ze swoich Umów i natychmiast otrzymać Dobro, które ona dostarcza.","cardType":6,"fractionType":0,"actionType":3,"contract":0,"cost":[6],"gain":[3,5],"image":57},</v>
       </c>
     </row>
@@ -3127,7 +3127,7 @@
         <v>58</v>
       </c>
       <c r="L59" t="str">
-        <f>_xlfn.CONCAT(B$1,B59,C$1,C59,D$1,D59,E$1,E59,F$1,F59,G$1,G59,H$1,H59,I$1,I59,J$1,J59,K$1,K59,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":58,"cardName":"MŁODNIK","description":"Akcja: Wydaj 1 #3, aby otrzymać 1 #7. Możesz aktywować ją dwa razy.","cardType":7,"fractionType":0,"actionType":3,"contract":0,"cost":[7],"gain":[7,7],"image":58},</v>
       </c>
     </row>
@@ -3166,7 +3166,7 @@
         <v>58</v>
       </c>
       <c r="L60" t="str">
-        <f>_xlfn.CONCAT(B$1,B60,C$1,C60,D$1,D60,E$1,E60,F$1,F60,G$1,G60,H$1,H60,I$1,I60,J$1,J60,K$1,K60,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":59,"cardName":"MŁODNIK","description":"Akcja: Wydaj 1 #3, aby otrzymać 1 #7. Możesz aktywować ją dwa razy.","cardType":7,"fractionType":0,"actionType":3,"contract":0,"cost":[7],"gain":[7,7],"image":58},</v>
       </c>
     </row>
@@ -3205,7 +3205,7 @@
         <v>58</v>
       </c>
       <c r="L61" t="str">
-        <f>_xlfn.CONCAT(B$1,B61,C$1,C61,D$1,D61,E$1,E61,F$1,F61,G$1,G61,H$1,H61,I$1,I61,J$1,J61,K$1,K61,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":60,"cardName":"MŁODNIK","description":"Akcja: Wydaj 1 #3, aby otrzymać 1 #7. Możesz aktywować ją dwa razy.","cardType":7,"fractionType":0,"actionType":3,"contract":0,"cost":[7],"gain":[7,7],"image":58},</v>
       </c>
     </row>
@@ -3244,7 +3244,7 @@
         <v>61</v>
       </c>
       <c r="L62" t="str">
-        <f>_xlfn.CONCAT(B$1,B62,C$1,C62,D$1,D62,E$1,E62,F$1,F62,G$1,G62,H$1,H62,I$1,I62,J$1,J62,K$1,K62,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":61,"cardName":"LIGA HANZEATYCKA","description":"Akcja: Wydaj 1 #3 oraz odrzuć 1 ze swoich umów, aby otrzymać 2 #2. Możesz aktywować ją dwa razy.","cardType":5,"fractionType":0,"actionType":3,"contract":0,"cost":[7,8,8],"gain":[2,5],"image":61},</v>
       </c>
     </row>
@@ -3283,7 +3283,7 @@
         <v>62</v>
       </c>
       <c r="L63" t="str">
-        <f>_xlfn.CONCAT(B$1,B63,C$1,C63,D$1,D63,E$1,E63,F$1,F63,G$1,G63,H$1,H63,I$1,I63,J$1,J63,K$1,K63,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":62,"cardName":"SZLAK DRWALI","description":"Produkcja: 1 #7. Bonus za zbudowanie: 1 #7","cardType":7,"fractionType":0,"actionType":1,"contract":0,"cost":[7,7],"gain":[7,7],"image":62},</v>
       </c>
     </row>
@@ -3322,7 +3322,7 @@
         <v>62</v>
       </c>
       <c r="L64" t="str">
-        <f>_xlfn.CONCAT(B$1,B64,C$1,C64,D$1,D64,E$1,E64,F$1,F64,G$1,G64,H$1,H64,I$1,I64,J$1,J64,K$1,K64,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":63,"cardName":"SZLAK DRWALI","description":"Produkcja: 1 #7. Bonus za zbudowanie: 1 #7","cardType":7,"fractionType":0,"actionType":1,"contract":0,"cost":[7,7],"gain":[7,7],"image":62},</v>
       </c>
     </row>
@@ -3361,7 +3361,7 @@
         <v>62</v>
       </c>
       <c r="L65" t="str">
-        <f>_xlfn.CONCAT(B$1,B65,C$1,C65,D$1,D65,E$1,E65,F$1,F65,G$1,G65,H$1,H65,I$1,I65,J$1,J65,K$1,K65,L$1)</f>
+        <f t="shared" si="1"/>
         <v>{"cardId":64,"cardName":"SZLAK DRWALI","description":"Produkcja: 1 #7. Bonus za zbudowanie: 1 #7","cardType":7,"fractionType":0,"actionType":1,"contract":0,"cost":[7,7],"gain":[7,7],"image":62},</v>
       </c>
     </row>
@@ -3400,7 +3400,7 @@
         <v>65</v>
       </c>
       <c r="L66" t="str">
-        <f>_xlfn.CONCAT(B$1,B66,C$1,C66,D$1,D66,E$1,E66,F$1,F66,G$1,G66,H$1,H66,I$1,I66,J$1,J66,K$1,K66,L$1)</f>
+        <f t="shared" ref="L66:L97" si="2">_xlfn.CONCAT(B$1,B66,C$1,C66,D$1,D66,E$1,E66,F$1,F66,G$1,G66,H$1,H66,I$1,I66,J$1,J66,K$1,K66,L$1)</f>
         <v>{"cardId":65,"cardName":"STRAŻNICA","description":"Produkcja: 1 #1. Bonus za zbudowanie: 1 #1.","cardType":1,"fractionType":0,"actionType":1,"contract":0,"cost":[7,7],"gain":[1,1],"image":65},</v>
       </c>
     </row>
@@ -3439,7 +3439,7 @@
         <v>65</v>
       </c>
       <c r="L67" t="str">
-        <f>_xlfn.CONCAT(B$1,B67,C$1,C67,D$1,D67,E$1,E67,F$1,F67,G$1,G67,H$1,H67,I$1,I67,J$1,J67,K$1,K67,L$1)</f>
+        <f t="shared" si="2"/>
         <v>{"cardId":66,"cardName":"STRAŻNICA","description":"Produkcja: 1 #1. Bonus za zbudowanie: 1 #1.","cardType":1,"fractionType":0,"actionType":1,"contract":0,"cost":[7,7],"gain":[1,1],"image":65},</v>
       </c>
     </row>
@@ -3478,7 +3478,7 @@
         <v>65</v>
       </c>
       <c r="L68" t="str">
-        <f>_xlfn.CONCAT(B$1,B68,C$1,C68,D$1,D68,E$1,E68,F$1,F68,G$1,G68,H$1,H68,I$1,I68,J$1,J68,K$1,K68,L$1)</f>
+        <f t="shared" si="2"/>
         <v>{"cardId":67,"cardName":"STRAŻNICA","description":"Produkcja: 1 #1. Bonus za zbudowanie: 1 #1.","cardType":1,"fractionType":0,"actionType":1,"contract":0,"cost":[7,7],"gain":[1,1],"image":65},</v>
       </c>
     </row>
@@ -3517,7 +3517,7 @@
         <v>65</v>
       </c>
       <c r="L69" t="str">
-        <f>_xlfn.CONCAT(B$1,B69,C$1,C69,D$1,D69,E$1,E69,F$1,F69,G$1,G69,H$1,H69,I$1,I69,J$1,J69,K$1,K69,L$1)</f>
+        <f t="shared" si="2"/>
         <v>{"cardId":68,"cardName":"STRAŻNICA","description":"Produkcja: 1 #1. Bonus za zbudowanie: 1 #1.","cardType":1,"fractionType":0,"actionType":1,"contract":0,"cost":[7,7],"gain":[1,1],"image":65},</v>
       </c>
     </row>
@@ -3550,7 +3550,7 @@
         <v>69</v>
       </c>
       <c r="L70" t="str">
-        <f>_xlfn.CONCAT(B$1,B70,C$1,C70,D$1,D70,E$1,E70,F$1,F70,G$1,G70,H$1,H70,I$1,I70,J$1,J70,K$1,K70,L$1)</f>
+        <f t="shared" si="2"/>
         <v>{"cardId":69,"cardName":"RUINY","description":"Cecha: -. Bonus za zbudowanie: 1 #3","cardType":9,"fractionType":0,"actionType":2,"contract":0,"cost":[],"gain":[],"image":69},</v>
       </c>
     </row>
@@ -3583,7 +3583,7 @@
         <v>69</v>
       </c>
       <c r="L71" t="str">
-        <f>_xlfn.CONCAT(B$1,B71,C$1,C71,D$1,D71,E$1,E71,F$1,F71,G$1,G71,H$1,H71,I$1,I71,J$1,J71,K$1,K71,L$1)</f>
+        <f t="shared" si="2"/>
         <v>{"cardId":70,"cardName":"RUINY","description":"Cecha: -. Bonus za zbudowanie: 1 #3","cardType":9,"fractionType":0,"actionType":2,"contract":0,"cost":[],"gain":[],"image":69},</v>
       </c>
     </row>
@@ -3616,7 +3616,7 @@
         <v>69</v>
       </c>
       <c r="L72" t="str">
-        <f>_xlfn.CONCAT(B$1,B72,C$1,C72,D$1,D72,E$1,E72,F$1,F72,G$1,G72,H$1,H72,I$1,I72,J$1,J72,K$1,K72,L$1)</f>
+        <f t="shared" si="2"/>
         <v>{"cardId":71,"cardName":"RUINY","description":"Cecha: -. Bonus za zbudowanie: 1 #3","cardType":9,"fractionType":0,"actionType":2,"contract":0,"cost":[],"gain":[],"image":69},</v>
       </c>
     </row>
@@ -3649,7 +3649,7 @@
         <v>69</v>
       </c>
       <c r="L73" t="str">
-        <f>_xlfn.CONCAT(B$1,B73,C$1,C73,D$1,D73,E$1,E73,F$1,F73,G$1,G73,H$1,H73,I$1,I73,J$1,J73,K$1,K73,L$1)</f>
+        <f t="shared" si="2"/>
         <v>{"cardId":72,"cardName":"RUINY","description":"Cecha: -. Bonus za zbudowanie: 1 #3","cardType":9,"fractionType":0,"actionType":2,"contract":0,"cost":[],"gain":[],"image":69},</v>
       </c>
     </row>
@@ -3682,7 +3682,7 @@
         <v>69</v>
       </c>
       <c r="L74" t="str">
-        <f>_xlfn.CONCAT(B$1,B74,C$1,C74,D$1,D74,E$1,E74,F$1,F74,G$1,G74,H$1,H74,I$1,I74,J$1,J74,K$1,K74,L$1)</f>
+        <f t="shared" si="2"/>
         <v>{"cardId":73,"cardName":"RUINY","description":"Cecha: -. Bonus za zbudowanie: 1 #3","cardType":9,"fractionType":0,"actionType":2,"contract":0,"cost":[],"gain":[],"image":69},</v>
       </c>
     </row>
@@ -3715,7 +3715,7 @@
         <v>69</v>
       </c>
       <c r="L75" t="str">
-        <f>_xlfn.CONCAT(B$1,B75,C$1,C75,D$1,D75,E$1,E75,F$1,F75,G$1,G75,H$1,H75,I$1,I75,J$1,J75,K$1,K75,L$1)</f>
+        <f t="shared" si="2"/>
         <v>{"cardId":74,"cardName":"RUINY","description":"Cecha: -. Bonus za zbudowanie: 1 #3","cardType":9,"fractionType":0,"actionType":2,"contract":0,"cost":[],"gain":[],"image":69},</v>
       </c>
     </row>
@@ -3754,7 +3754,7 @@
         <v>75</v>
       </c>
       <c r="L76" t="str">
-        <f>_xlfn.CONCAT(B$1,B76,C$1,C76,D$1,D76,E$1,E76,F$1,F76,G$1,G76,H$1,H76,I$1,I76,J$1,J76,K$1,K76,L$1)</f>
+        <f t="shared" si="2"/>
         <v>{"cardId":75,"cardName":"PIEKARZ","description":"Cecha: - . Bonus za zbudowanie: 1 #2 za każdą CZERWONĄ #9 w twoim imperium, maks 6. Dodatkowo dobierz 1 #1.","cardType":6,"fractionType":0,"actionType":2,"contract":0,"cost":[7,7,8],"gain":[2,6],"image":75},</v>
       </c>
     </row>
@@ -3793,7 +3793,7 @@
         <v>76</v>
       </c>
       <c r="L77" t="str">
-        <f>_xlfn.CONCAT(B$1,B77,C$1,C77,D$1,D77,E$1,E77,F$1,F77,G$1,G77,H$1,H77,I$1,I77,J$1,J77,K$1,K77,L$1)</f>
+        <f t="shared" si="2"/>
         <v>{"cardId":76,"cardName":"TARTAK","description":"Akcja: Wydaj 1 #7, aby otrzymać 1 #2. Możesz aktywować ją dwa razy.","cardType":7,"fractionType":0,"actionType":3,"contract":0,"cost":[7],"gain":[3,7],"image":76},</v>
       </c>
     </row>
@@ -3832,7 +3832,7 @@
         <v>76</v>
       </c>
       <c r="L78" t="str">
-        <f>_xlfn.CONCAT(B$1,B78,C$1,C78,D$1,D78,E$1,E78,F$1,F78,G$1,G78,H$1,H78,I$1,I78,J$1,J78,K$1,K78,L$1)</f>
+        <f t="shared" si="2"/>
         <v>{"cardId":77,"cardName":"TARTAK","description":"Akcja: Wydaj 1 #7, aby otrzymać 1 #2. Możesz aktywować ją dwa razy.","cardType":7,"fractionType":0,"actionType":3,"contract":0,"cost":[7],"gain":[3,7],"image":76},</v>
       </c>
     </row>
@@ -3871,7 +3871,7 @@
         <v>78</v>
       </c>
       <c r="L79" t="str">
-        <f>_xlfn.CONCAT(B$1,B79,C$1,C79,D$1,D79,E$1,E79,F$1,F79,G$1,G79,H$1,H79,I$1,I79,J$1,J79,K$1,K79,L$1)</f>
+        <f t="shared" si="2"/>
         <v>{"cardId":78,"cardName":"KANTYNA","description":"Cecha: Zawsze gdy zbudujesz RÓŻOWĄ #9, otrzymujesz 1 #5 i 1 #2.","cardType":3,"fractionType":0,"actionType":2,"contract":0,"cost":[7,7,7],"gain":[3,6],"image":78},</v>
       </c>
     </row>
@@ -3910,7 +3910,7 @@
         <v>79</v>
       </c>
       <c r="L80" t="str">
-        <f>_xlfn.CONCAT(B$1,B80,C$1,C80,D$1,D80,E$1,E80,F$1,F80,G$1,G80,H$1,H80,I$1,I80,J$1,J80,K$1,K80,L$1)</f>
+        <f t="shared" si="2"/>
         <v>{"cardId":79,"cardName":"MIEJSCE ZGROMADZEŃ","description":"Cecha: - . Bonus za zbudowanie: 1 #2 za każdą RÓŻOWĄ #9 w twoim imperium, maks 6. Dodatkowo dobierz 1 #1.","cardType":3,"fractionType":0,"actionType":2,"contract":0,"cost":[7,7,8],"gain":[3,1],"image":79},</v>
       </c>
     </row>
@@ -3949,7 +3949,7 @@
         <v>80</v>
       </c>
       <c r="L81" t="str">
-        <f>_xlfn.CONCAT(B$1,B81,C$1,C81,D$1,D81,E$1,E81,F$1,F81,G$1,G81,H$1,H81,I$1,I81,J$1,J81,K$1,K81,L$1)</f>
+        <f t="shared" si="2"/>
         <v>{"cardId":80,"cardName":"KUPIEC BOGDAN","description":"Cecha: Zawsze gdy zbudujesz ZŁOTĄ #9, otrzymasz 1 #5 i 1 #2.","cardType":5,"fractionType":0,"actionType":2,"contract":0,"cost":[7,8,8],"gain":[5,8],"image":80},</v>
       </c>
     </row>
@@ -3988,7 +3988,7 @@
         <v>81</v>
       </c>
       <c r="L82" t="str">
-        <f>_xlfn.CONCAT(B$1,B82,C$1,C82,D$1,D82,E$1,E82,F$1,F82,G$1,G82,H$1,H82,I$1,I82,J$1,J82,K$1,K82,L$1)</f>
+        <f t="shared" si="2"/>
         <v>{"cardId":81,"cardName":"APARTAMENTY","description":"Cecha: - . Bonus za zbudowanie: 1 #2 za każdą ZŁOTĄ #9 w twoim imperium, maks 6. Dodatkowo dobierz 1 #1.","cardType":5,"fractionType":0,"actionType":2,"contract":0,"cost":[7,8,8],"gain":[5,8],"image":81},</v>
       </c>
     </row>
@@ -4027,7 +4027,7 @@
         <v>82</v>
       </c>
       <c r="L83" t="str">
-        <f>_xlfn.CONCAT(B$1,B83,C$1,C83,D$1,D83,E$1,E83,F$1,F83,G$1,G83,H$1,H83,I$1,I83,J$1,J83,K$1,K83,L$1)</f>
+        <f t="shared" si="2"/>
         <v>{"cardId":82,"cardName":"MYŚLIWY JÓZEK","description":"Akcja: Wydaj 1 #3, aby otrzymać 2 #6.","cardType":6,"fractionType":0,"actionType":3,"contract":0,"cost":[7],"gain":[7,6],"image":82},</v>
       </c>
     </row>
@@ -4066,7 +4066,7 @@
         <v>83</v>
       </c>
       <c r="L84" t="str">
-        <f>_xlfn.CONCAT(B$1,B84,C$1,C84,D$1,D84,E$1,E84,F$1,F84,G$1,G84,H$1,H84,I$1,I84,J$1,J84,K$1,K84,L$1)</f>
+        <f t="shared" si="2"/>
         <v>{"cardId":83,"cardName":"KOPALNIA ODKRYWKOWA","description":"Akcja: Wydaj 1 #3, aby otrzymać 1 #8. Możesz aktywować ją dwa razy.","cardType":8,"fractionType":0,"actionType":3,"contract":0,"cost":[8],"gain":[8,8],"image":83},</v>
       </c>
     </row>
@@ -4105,7 +4105,7 @@
         <v>84</v>
       </c>
       <c r="L85" t="str">
-        <f>_xlfn.CONCAT(B$1,B85,C$1,C85,D$1,D85,E$1,E85,F$1,F85,G$1,G85,H$1,H85,I$1,I85,J$1,J85,K$1,K85,L$1)</f>
+        <f t="shared" si="2"/>
         <v>{"cardId":84,"cardName":"TRAGARZE","description":"Akcja: Wydaj 1 #6, aby wybrać dowolną ze swoich #9 PRODUKCYJNYCH i orzymaj Dobra, których ona dostarcza.","cardType":3,"fractionType":0,"actionType":3,"contract":0,"cost":[7,7],"gain":[3,8],"image":84},</v>
       </c>
     </row>

</xml_diff>